<commit_message>
refine the xlsx file format
</commit_message>
<xml_diff>
--- a/漫展信息/广州-漫展信息.xlsx
+++ b/漫展信息/广州-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,25 +457,30 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>单程耗时</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>具体时间范围</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>想去人数</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>最低票价</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>是否有舞台（字符串匹配）</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -492,31 +497,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>广州·第五届清云动漫展</t>
+          <t>广州·运动番ONLY</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>丰乐北路898号 雅居乐黄埔创新中心</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
         <is>
           <t>2024.01.20 10:00-01.20 17:00</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>69</v>
-      </c>
       <c r="G2" t="n">
-        <v>40</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80502&amp;msource=Msearch_colligation</t>
+        <v>1194</v>
+      </c>
+      <c r="H2" t="n">
+        <v>60</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=77532&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -526,36 +532,39 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024.01.20</t>
+          <t>2024.01.21</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>广州·运动番ONLY</t>
+          <t>广州·全职高手only（取消）</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1043</v>
+          <t>鹤龙街道 鹤边鹤龙二横街3号D栋2楼 T20视觉艺术空间</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024.01.21 10:00-01.21 17:00</t>
+        </is>
       </c>
       <c r="G3" t="n">
-        <v>60</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77532&amp;msource=Msearch_colligation</t>
+        <v>121</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80210&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -565,38 +574,39 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024.01.21</t>
+          <t>2024.01.26</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>广州·全职高手only（取消）</t>
+          <t>广州·《FGO》FES2024·广州特别纪念展</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>鹤龙街道 鹤边鹤龙二横街3号D栋2楼 T20视觉艺术空间</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024.01.21 10:00-01.21 17:00</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>121</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>不可售</t>
-        </is>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80210&amp;msource=Msearch_colligation</t>
+          <t>新港东路1000号 保利世贸博览馆</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024.01.26 09:00-01.28 17:00</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>11218</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>已售罄</t>
+        </is>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80066&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -606,38 +616,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024.01.26</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>广州·《FGO》FES2024·广州特别纪念展</t>
+          <t>广州.星火.AI次元动漫展</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>新港东路1000号 保利世贸博览馆</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024.01.26 09:00-01.28 17:00</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>11084</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>已售罄</t>
-        </is>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80066&amp;msource=Msearch_colligation</t>
+          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024.01.27 10:00-01.27 17:00</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>1534</v>
+      </c>
+      <c r="H5" t="n">
+        <v>55</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78754&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -652,31 +661,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>广州.星火.AI次元动漫展</t>
+          <t>广州·妖都魔法少女小圆ONLY</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+          <t>同泰路颐和山庄内国际会议厅 颐和山庄</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
         <is>
           <t>2024.01.27 10:00-01.27 17:00</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>1243</v>
-      </c>
       <c r="G6" t="n">
-        <v>55</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78754&amp;msource=Msearch_colligation</t>
+        <v>429</v>
+      </c>
+      <c r="H6" t="n">
+        <v>68</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79748&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -691,31 +701,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>广州·妖都魔法少女小圆ONLY</t>
+          <t>广州·第七届萌物语动漫嘉年华</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>同泰路颐和山庄内国际会议厅 颐和山庄</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
+          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
         <is>
           <t>2024.01.27 10:00-01.27 17:00</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>381</v>
-      </c>
       <c r="G7" t="n">
-        <v>68</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79748&amp;msource=Msearch_colligation</t>
+        <v>705</v>
+      </c>
+      <c r="H7" t="n">
+        <v>60</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79317&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -730,31 +741,34 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>广州·第七届萌物语动漫嘉年华</t>
+          <t>广州·第五人格only唐人街春市</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2024.01.27 10:00-01.27 17:00</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>619</v>
+          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024.01.27 10:00-01.27 16:30</t>
+        </is>
       </c>
       <c r="G8" t="n">
-        <v>60</v>
-      </c>
-      <c r="H8" t="b">
+        <v>2195</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
+      </c>
+      <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79317&amp;msource=Msearch_colligation</t>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79038&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -769,33 +783,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>广州·第五人格only唐人街春市</t>
+          <t>广州·第五届ACBC动漫盛典-二次元游园会</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2024.01.27 10:00-01.27 16:30</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>2033</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>不可售</t>
-        </is>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79038&amp;msource=Msearch_colligation</t>
+          <t>沙滘中路41-50号 火星工厂</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024.01.27 12:00-01.29 00:00</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>646</v>
+      </c>
+      <c r="H9" t="n">
+        <v>48</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80415&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -810,31 +823,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>广州·第五届ACBC动漫盛典-二次元游园会</t>
+          <t>广州·蓝锁only2.0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>沙滘中路41-50号 火星工厂</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2024.01.27 12:00-01.29 00:00</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>606</v>
+          <t>大石街石北工业大道644号 巨大创意产业园</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024.01.27 10:00-01.27 17:00</t>
+        </is>
       </c>
       <c r="G10" t="n">
-        <v>48</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80415&amp;msource=Msearch_colligation</t>
+        <v>865</v>
+      </c>
+      <c r="H10" t="n">
+        <v>65</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79750&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -844,36 +858,37 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024.01.27</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>广州·蓝锁only2.0</t>
+          <t>广州·文豪野犬only</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>大石街石北工业大道644号 巨大创意产业园</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2024.01.27 10:00-01.27 17:00</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>757</v>
+          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024.01.28 10:00-01.28 17:00</t>
+        </is>
       </c>
       <c r="G11" t="n">
-        <v>65</v>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79750&amp;msource=Msearch_colligation</t>
+        <v>467</v>
+      </c>
+      <c r="H11" t="n">
+        <v>60</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80436&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -883,7 +898,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.01.29</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,21 +911,22 @@
           <t>奥体南路12号 优托邦(奥体旗舰店)</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2024.01.28 10:00-01.28 17:00</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>247</v>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2024.01.29 10:00-01.29 17:00</t>
+        </is>
       </c>
       <c r="G12" t="n">
+        <v>345</v>
+      </c>
+      <c r="H12" t="n">
         <v>60</v>
       </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80453&amp;msource=Msearch_colligation</t>
         </is>
@@ -922,12 +938,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.01.30</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>广州·文豪野犬only</t>
+          <t>广州·进击的巨人only</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -935,23 +951,24 @@
           <t>奥体南路12号 优托邦(奥体旗舰店)</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2024.01.28 10:00-01.28 17:00</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>332</v>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024.01.30 10:00-01.30 17:00</t>
+        </is>
       </c>
       <c r="G13" t="n">
+        <v>381</v>
+      </c>
+      <c r="H13" t="n">
         <v>60</v>
       </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80436&amp;msource=Msearch_colligation</t>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80454&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -961,36 +978,37 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024.01.30</t>
+          <t>2024.02.01</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>广州·进击的巨人only</t>
+          <t>广州·U.M.A闪耀ONLY（马娘only）</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2024.01.30 10:00-01.30 17:00</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>310</v>
+          <t>东圃中山大道中358号 轰谧斯酒店</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2024.02.01 10:00-02.01 17:00</t>
+        </is>
       </c>
       <c r="G14" t="n">
-        <v>60</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80454&amp;msource=Msearch_colligation</t>
+        <v>351</v>
+      </c>
+      <c r="H14" t="n">
+        <v>68</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80184&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1000,36 +1018,37 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024.02.01</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>广州·U.M.A闪耀ONLY（马娘only）</t>
+          <t>从化·FS动漫展</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>东圃中山大道中358号 轰谧斯酒店</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2024.02.01 10:00-02.01 17:00</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>292</v>
+          <t>从城大道383号 云岭湖酒店</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2024.02.03 10:00-02.03 17:00</t>
+        </is>
       </c>
       <c r="G15" t="n">
-        <v>68</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80184&amp;msource=Msearch_colligation</t>
+        <v>1118</v>
+      </c>
+      <c r="H15" t="n">
+        <v>35</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=77976&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1044,31 +1063,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>从化·FS动漫展</t>
+          <t>广州·怀旧ONLY</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>从城大道383号 云岭湖酒店</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2024.02.03 10:00-02.03 17:00</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>1025</v>
+          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2024.02.03 10:00-02.03 16:30</t>
+        </is>
       </c>
       <c r="G16" t="n">
-        <v>35</v>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77976&amp;msource=Msearch_colligation</t>
+        <v>489</v>
+      </c>
+      <c r="H16" t="n">
+        <v>60</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79752&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1078,36 +1098,37 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024.02.03</t>
+          <t>2024.02.12</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>广州·怀旧ONLY</t>
+          <t>广州·EY动漫嘉年华</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2024.02.03 10:00-02.03 16:30</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>398</v>
+          <t>机场路1399号广州百信广场二期 李宁运动中心</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2024.02.12 10:00-02.12 17:00</t>
+        </is>
       </c>
       <c r="G17" t="n">
-        <v>75</v>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79752&amp;msource=Msearch_colligation</t>
+        <v>872</v>
+      </c>
+      <c r="H17" t="n">
+        <v>63</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80574&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1117,36 +1138,37 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024.02.12</t>
+          <t>2024.02.14</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>广州·EY动漫嘉年华</t>
+          <t>广州·运动番only4.0</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>机场路1399号广州百信广场二期 李宁运动中心</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2024.02.12 10:00-02.12 17:00</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>95</v>
+          <t>洛浦街厦滘西环路1号 岭南会展中心</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2024.02.14 10:00-02.14 17:00</t>
+        </is>
       </c>
       <c r="G18" t="n">
-        <v>63</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80574&amp;msource=Msearch_colligation</t>
+        <v>338</v>
+      </c>
+      <c r="H18" t="n">
+        <v>60</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80499&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1156,12 +1178,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024.02.14</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>广州·运动番only4.0</t>
+          <t>广州· 妖都原神only 2.0-提瓦特新春游园会</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1169,23 +1191,24 @@
           <t>洛浦街厦滘西环路1号 岭南会展中心</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2024.02.14 10:00-02.14 17:00</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>223</v>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2024.02.16 09:30-02.16 16:30</t>
+        </is>
       </c>
       <c r="G19" t="n">
-        <v>60</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80499&amp;msource=Msearch_colligation</t>
+        <v>523</v>
+      </c>
+      <c r="H19" t="n">
+        <v>58</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79914&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1200,31 +1223,32 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>广州· 妖都原神only 2.0-提瓦特新春游园会</t>
+          <t>广州·樱漫动漫嘉年华8.0</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>洛浦街厦滘西环路1号 岭南会展中心</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2024.02.16 09:30-02.16 16:30</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>457</v>
+          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2024.02.16 10:00-02.17 17:00</t>
+        </is>
       </c>
       <c r="G20" t="n">
+        <v>823</v>
+      </c>
+      <c r="H20" t="n">
         <v>58</v>
       </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79914&amp;msource=Msearch_colligation</t>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79792&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1234,36 +1258,37 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.18</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>广州·樱漫动漫嘉年华8.0</t>
+          <t>广州·cooperative kingdom同人展2.0</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2024.02.16 10:00-02.17 17:00</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>685</v>
+          <t>洛浦街夏滘西环路1号 岭南电商园</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2024.02.18 10:00-02.18 17:00</t>
+        </is>
       </c>
       <c r="G21" t="n">
-        <v>58</v>
-      </c>
-      <c r="H21" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79792&amp;msource=Msearch_colligation</t>
+        <v>847</v>
+      </c>
+      <c r="H21" t="n">
+        <v>55</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79264&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1273,36 +1298,37 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024.02.18</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>广州·cooperative kingdom同人展2.0</t>
+          <t>广州·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>洛浦街夏滘西环路1号 岭南电商园</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2024.02.18 10:00-02.18 17:00</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>801</v>
+          <t>西湾路150号 悦汇城</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2024.02.24 13:00-02.25 19:00</t>
+        </is>
       </c>
       <c r="G22" t="n">
-        <v>55</v>
-      </c>
-      <c r="H22" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79264&amp;msource=Msearch_colligation</t>
+        <v>66</v>
+      </c>
+      <c r="H22" t="n">
+        <v>48</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80624&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1317,31 +1343,32 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>广州·SISP动漫游戏嘉年华</t>
+          <t>广州·砂糖桔动漫荟STJ01</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>西湾路150号 悦汇城</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>10</v>
+          <t>东沙大道16号 广州国际医药港</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2024.02.24 10:00-02.25 18:00</t>
+        </is>
       </c>
       <c r="G23" t="n">
-        <v>48</v>
-      </c>
-      <c r="H23" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80624&amp;msource=Msearch_colligation</t>
+        <v>87</v>
+      </c>
+      <c r="H23" t="n">
+        <v>60</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80774&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1351,36 +1378,37 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024.03.02</t>
+          <t>2024.02.25</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>广州·明日方舟ONLY</t>
+          <t>广州·第五届清云动漫展</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>清河东路288号 科尔海悦酒店</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2024.03.02 10:00-03.02 17:00</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>185</v>
+          <t>丰乐北路898号 雅居乐黄埔创新中心</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2024.02.25 10:00-02.25 17:00</t>
+        </is>
       </c>
       <c r="G24" t="n">
-        <v>60</v>
-      </c>
-      <c r="H24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80271&amp;msource=Msearch_colligation</t>
+        <v>90</v>
+      </c>
+      <c r="H24" t="n">
+        <v>40</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80502&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1390,12 +1418,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024.03.16</t>
+          <t>2024.03.02</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>广州·代号鸢only2.0</t>
+          <t>广州·明日方舟ONLY</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1403,23 +1431,24 @@
           <t>清河东路288号 科尔海悦酒店</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>2024.03.16 10:00-03.16 21:00</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>474</v>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2024.03.02 10:00-03.02 17:00</t>
+        </is>
       </c>
       <c r="G25" t="n">
-        <v>39</v>
-      </c>
-      <c r="H25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79828&amp;msource=Msearch_colligation</t>
+        <v>220</v>
+      </c>
+      <c r="H25" t="n">
+        <v>60</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80271&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1434,31 +1463,32 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>广州·原神X星穹铁道X绝区零ONLY</t>
+          <t>广州·代号鸢only2.0</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>洛浦街夏滘西环路1号(厦滘地铁站A口步行290米) 厦喾岭南电商园会展中心</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>2024.03.16 10:00-03.16 17:00</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>1</v>
+          <t>清河东路288号 科尔海悦酒店</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2024.03.16 10:00-03.16 21:00</t>
+        </is>
       </c>
       <c r="G26" t="n">
-        <v>60</v>
-      </c>
-      <c r="H26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80715&amp;msource=Msearch_colligation</t>
+        <v>553</v>
+      </c>
+      <c r="H26" t="n">
+        <v>39</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79828&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1468,36 +1498,37 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024.03.23</t>
+          <t>2024.03.16</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>广州·排球少年ONLY</t>
+          <t>广州·原神X星穹铁道X绝区零ONLY</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>机场路1399号广州百信广场二期 李宁运动中心</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2024.03.23 10:00-03.23 17:00</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
+          <t>洛浦街夏滘西环路1号(厦滘地铁站A口步行290米) 厦喾岭南电商园会展中心</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2024.03.16 10:00-03.16 17:00</t>
+        </is>
       </c>
       <c r="G27" t="n">
+        <v>80</v>
+      </c>
+      <c r="H27" t="n">
         <v>60</v>
       </c>
-      <c r="H27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80716&amp;msource=Msearch_colligation</t>
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80715&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1507,36 +1538,37 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024.04.20</t>
+          <t>2024.03.23</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>广州·Arknights Only·夜航星（明日方舟Only)</t>
+          <t>广州·排球少年ONLY</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>同泰路颐和山庄 颐和大酒店</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>2024.04.20 10:00-04.20 17:00</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>217</v>
+          <t>机场路1399号广州百信广场二期 李宁运动中心</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2024.03.23 10:00-03.23 17:00</t>
+        </is>
       </c>
       <c r="G28" t="n">
-        <v>69</v>
-      </c>
-      <c r="H28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80282&amp;msource=Msearch_colligation</t>
+        <v>33</v>
+      </c>
+      <c r="H28" t="n">
+        <v>60</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80716&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1544,14 +1576,41 @@
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2024.04.20</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>广州·Arknights Only·夜航星（明日方舟Only)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>同泰路颐和山庄 颐和大酒店</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2024.04.20 10:00-04.20 17:00</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>266</v>
+      </c>
+      <c r="H29" t="n">
+        <v>69</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80282&amp;msource=Msearch_colligation</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1565,17 +1624,13 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>数据来自B站会员购，仅供学习交流用途，严禁商业用途
-项目地址：https://github.com/zxcsjf/BilibiliAnimationExhibitionInformationCollection</t>
-        </is>
-      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="inlineStr"/>
@@ -1583,6 +1638,26 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>数据来自B站会员购，仅供学习交流用途，严禁商业用途
+项目地址：https://github.com/zxcsjf/BilibiliAnimationExhibitionInformationCollection</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1595,7 +1670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1624,25 +1699,30 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>单程耗时</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>具体时间范围</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>想去人数</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>最低票价</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>是否有舞台（字符串匹配）</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -1654,36 +1734,39 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024.01.14</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">广州·【限时7折】“阿根廷瑰宝”舞中之王-探戈舞剧《燃情探戈》 </t>
+          <t xml:space="preserve">广州· 西班牙格拉纳达弗拉门戈舞团经典舞剧《卡门》 白金版  </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>人民北路696号 广州友谊剧院</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024.01.14 19:30-01.14 21:00</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
+          <t>中山纪念堂 中山纪念堂</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024.01.20 20:00-01.20 21:40</t>
+        </is>
       </c>
       <c r="G2" t="n">
-        <v>280</v>
-      </c>
-      <c r="H2" t="b">
+        <v>66</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
+      </c>
+      <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78417&amp;msource=Msearch_colligation</t>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=74796&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1693,38 +1776,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024.01.20</t>
+          <t>2024.01.21</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">广州· 西班牙格拉纳达弗拉门戈舞团经典舞剧《卡门》 白金版  </t>
+          <t xml:space="preserve">广州·Ayasa LIVE TOUR 2024 〜A fraction〜 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>中山纪念堂 中山纪念堂</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024.01.20 20:00-01.20 21:40</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>66</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>不可售</t>
-        </is>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=74796&amp;msource=Msearch_colligation</t>
+          <t>海珠同创汇东一街11号（上冲南约11-2） 声音共和Livehouse</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024.01.21 15:30-01.21 17:00</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>685</v>
+      </c>
+      <c r="H3" t="n">
+        <v>380</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79174&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1739,31 +1821,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">广州·Ayasa LIVE TOUR 2024 〜A fraction〜 </t>
+          <t>广州·青春国乐进行时——方锦龙和他的弟子们国潮音乐会</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>海珠同创汇东一街11号（上冲南约11-2） 声音共和Livehouse</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024.01.21 15:30-01.21 17:00</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>649</v>
+          <t>中山纪念堂 中山纪念堂</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024.01.21 19:30-01.21 21:00</t>
+        </is>
       </c>
       <c r="G4" t="n">
-        <v>380</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79174&amp;msource=Msearch_colligation</t>
+        <v>30</v>
+      </c>
+      <c r="H4" t="n">
+        <v>180</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79170&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1773,36 +1856,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024.01.21</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>广州·青春国乐进行时——方锦龙和他的弟子们国潮音乐会</t>
+          <t>广州·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>中山纪念堂 中山纪念堂</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024.01.21 19:30-01.21 21:00</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>27</v>
+          <t>恩宁路265号三层、四层自编01 MAO Livehouse广州(永庆坊店)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024.01.27 20:00-01.27 22:00</t>
+        </is>
       </c>
       <c r="G5" t="n">
-        <v>180</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79170&amp;msource=Msearch_colligation</t>
+        <v>71</v>
+      </c>
+      <c r="H5" t="n">
+        <v>380</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79638&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1812,36 +1896,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024.01.27</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>广州·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>广州·《卡农》世界经典音乐之旅音乐会</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>恩宁路265号三层、四层自编01 MAO Livehouse广州(永庆坊店)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2024.01.27 20:00-01.27 22:00</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>62</v>
+          <t>东风中路299号 广州中山纪念堂</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024.01.28 19:00-01.28 21:00</t>
+        </is>
       </c>
       <c r="G6" t="n">
-        <v>380</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79638&amp;msource=Msearch_colligation</t>
+        <v>26</v>
+      </c>
+      <c r="H6" t="n">
+        <v>100</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80047&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1851,36 +1936,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.02.04</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>广州·《卡农》世界经典音乐之旅音乐会</t>
+          <t>广州·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>东风中路299号 广州中山纪念堂</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2024.01.28 19:00-01.28 21:00</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>20</v>
+          <t>革新路124号 太古仓码头</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024.02.04 12:30-02.04 21:00</t>
+        </is>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80047&amp;msource=Msearch_colligation</t>
+        <v>760</v>
+      </c>
+      <c r="H7" t="n">
+        <v>380</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80147&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1890,36 +1976,37 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024.02.04</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>广州·次元LAB 二次元电音节</t>
+          <t>广州黄龄【有没有吃过饭】LIVEHOUSE巡演—广州站</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>革新路124号 太古仓码头</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2024.02.04 12:30-02.04 21:00</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>661</v>
+          <t>新港东路磨碟沙大街118号第8栋 媒棚LIVE</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024.02.24 20:00-02.24 22:00</t>
+        </is>
       </c>
       <c r="G8" t="n">
-        <v>380</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80147&amp;msource=Msearch_colligation</t>
+        <v>13</v>
+      </c>
+      <c r="H8" t="n">
+        <v>420</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80205&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -1927,40 +2014,15 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2024.02.24</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>广州黄龄【有没有吃过饭】LIVEHOUSE巡演—广州站</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>新港东路磨碟沙大街118号第8栋 媒棚LIVE</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2024.02.24 20:00-02.24 22:00</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" t="n">
-        <v>420</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80205&amp;msource=Msearch_colligation</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1974,12 +2036,18 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>数据来自B站会员购，仅供学习交流用途，严禁商业用途
+项目地址：https://github.com/zxcsjf/BilibiliAnimationExhibitionInformationCollection</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
@@ -1987,24 +2055,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>数据来自B站会员购，仅供学习交流用途，严禁商业用途
-项目地址：https://github.com/zxcsjf/BilibiliAnimationExhibitionInformationCollection</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2017,7 +2068,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2046,25 +2097,30 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>单程耗时</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>具体时间范围</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>想去人数</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>最低票价</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>是否有舞台（字符串匹配）</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -2082,6 +2138,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2095,6 +2152,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2113,6 +2171,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2125,7 +2184,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2154,25 +2213,30 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>单程耗时</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>具体时间范围</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>想去人数</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>最低票价</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>是否有舞台（字符串匹配）</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -2184,36 +2248,39 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024.01.14</t>
+          <t>2024.01.20</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">广州·【限时7折】“阿根廷瑰宝”舞中之王-探戈舞剧《燃情探戈》 </t>
+          <t xml:space="preserve">广州· 西班牙格拉纳达弗拉门戈舞团经典舞剧《卡门》 白金版  </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>人民北路696号 广州友谊剧院</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024.01.14 19:30-01.14 21:00</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
+          <t>中山纪念堂 中山纪念堂</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2024.01.20 20:00-01.20 21:40</t>
+        </is>
       </c>
       <c r="G2" t="n">
-        <v>280</v>
-      </c>
-      <c r="H2" t="b">
+        <v>66</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
+      </c>
+      <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78417&amp;msource=Msearch_colligation</t>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=74796&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2228,33 +2295,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">广州· 西班牙格拉纳达弗拉门戈舞团经典舞剧《卡门》 白金版  </t>
+          <t>广州·运动番ONLY</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>中山纪念堂 中山纪念堂</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024.01.20 20:00-01.20 21:40</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>66</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>不可售</t>
-        </is>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=74796&amp;msource=Msearch_colligation</t>
+          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024.01.20 10:00-01.20 17:00</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1194</v>
+      </c>
+      <c r="H3" t="n">
+        <v>60</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=77532&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2264,36 +2330,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024.01.20</t>
+          <t>2024.01.21</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>广州·第五届清云动漫展</t>
+          <t xml:space="preserve">广州·Ayasa LIVE TOUR 2024 〜A fraction〜 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>丰乐北路898号 雅居乐黄埔创新中心</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>69</v>
+          <t>海珠同创汇东一街11号（上冲南约11-2） 声音共和Livehouse</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024.01.21 15:30-01.21 17:00</t>
+        </is>
       </c>
       <c r="G4" t="n">
-        <v>40</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80502&amp;msource=Msearch_colligation</t>
+        <v>685</v>
+      </c>
+      <c r="H4" t="n">
+        <v>380</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79174&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2303,36 +2370,39 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024.01.20</t>
+          <t>2024.01.21</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>广州·运动番ONLY</t>
+          <t>广州·全职高手only（取消）</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2024.01.20 10:00-01.20 17:00</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>1043</v>
+          <t>鹤龙街道 鹤边鹤龙二横街3号D栋2楼 T20视觉艺术空间</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024.01.21 10:00-01.21 17:00</t>
+        </is>
       </c>
       <c r="G5" t="n">
-        <v>60</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77532&amp;msource=Msearch_colligation</t>
+        <v>121</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80210&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2347,31 +2417,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">广州·Ayasa LIVE TOUR 2024 〜A fraction〜 </t>
+          <t>广州·青春国乐进行时——方锦龙和他的弟子们国潮音乐会</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>海珠同创汇东一街11号（上冲南约11-2） 声音共和Livehouse</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2024.01.21 15:30-01.21 17:00</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>649</v>
+          <t>中山纪念堂 中山纪念堂</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024.01.21 19:30-01.21 21:00</t>
+        </is>
       </c>
       <c r="G6" t="n">
-        <v>380</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79174&amp;msource=Msearch_colligation</t>
+        <v>30</v>
+      </c>
+      <c r="H6" t="n">
+        <v>180</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79170&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2381,38 +2452,39 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024.01.21</t>
+          <t>2024.01.26</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>广州·全职高手only（取消）</t>
+          <t>广州·《FGO》FES2024·广州特别纪念展</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>鹤龙街道 鹤边鹤龙二横街3号D栋2楼 T20视觉艺术空间</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2024.01.21 10:00-01.21 17:00</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>121</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>不可售</t>
-        </is>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80210&amp;msource=Msearch_colligation</t>
+          <t>新港东路1000号 保利世贸博览馆</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024.01.26 09:00-01.28 17:00</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>11218</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>已售罄</t>
+        </is>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80066&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2422,36 +2494,37 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024.01.21</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>广州·青春国乐进行时——方锦龙和他的弟子们国潮音乐会</t>
+          <t>广州.星火.AI次元动漫展</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>中山纪念堂 中山纪念堂</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2024.01.21 19:30-01.21 21:00</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>27</v>
+          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024.01.27 10:00-01.27 17:00</t>
+        </is>
       </c>
       <c r="G8" t="n">
-        <v>180</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79170&amp;msource=Msearch_colligation</t>
+        <v>1534</v>
+      </c>
+      <c r="H8" t="n">
+        <v>55</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78754&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2461,38 +2534,37 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024.01.26</t>
+          <t>2024.01.27</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>广州·《FGO》FES2024·广州特别纪念展</t>
+          <t>广州·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>新港东路1000号 保利世贸博览馆</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2024.01.26 09:00-01.28 17:00</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>11084</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>已售罄</t>
-        </is>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80066&amp;msource=Msearch_colligation</t>
+          <t>恩宁路265号三层、四层自编01 MAO Livehouse广州(永庆坊店)</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024.01.27 20:00-01.27 22:00</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>71</v>
+      </c>
+      <c r="H9" t="n">
+        <v>380</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79638&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2507,31 +2579,32 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>广州.星火.AI次元动漫展</t>
+          <t>广州·妖都魔法少女小圆ONLY</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+          <t>同泰路颐和山庄内国际会议厅 颐和山庄</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
         <is>
           <t>2024.01.27 10:00-01.27 17:00</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>1243</v>
-      </c>
       <c r="G10" t="n">
-        <v>55</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78754&amp;msource=Msearch_colligation</t>
+        <v>429</v>
+      </c>
+      <c r="H10" t="n">
+        <v>68</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79748&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2546,31 +2619,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>广州·七音阿卡莉 NANAOAKARI 2024 专场演出</t>
+          <t>广州·第七届萌物语动漫嘉年华</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>恩宁路265号三层、四层自编01 MAO Livehouse广州(永庆坊店)</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2024.01.27 20:00-01.27 22:00</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>62</v>
+          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024.01.27 10:00-01.27 17:00</t>
+        </is>
       </c>
       <c r="G11" t="n">
-        <v>380</v>
-      </c>
-      <c r="H11" t="b">
+        <v>705</v>
+      </c>
+      <c r="H11" t="n">
+        <v>60</v>
+      </c>
+      <c r="I11" t="b">
         <v>1</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79638&amp;msource=Msearch_colligation</t>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79317&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2585,31 +2659,34 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>广州·妖都魔法少女小圆ONLY</t>
+          <t>广州·第五人格only唐人街春市</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>同泰路颐和山庄内国际会议厅 颐和山庄</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2024.01.27 10:00-01.27 17:00</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>381</v>
+          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2024.01.27 10:00-01.27 16:30</t>
+        </is>
       </c>
       <c r="G12" t="n">
-        <v>68</v>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79748&amp;msource=Msearch_colligation</t>
+        <v>2195</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>不可售</t>
+        </is>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79038&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2624,31 +2701,32 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>广州·第七届萌物语动漫嘉年华</t>
+          <t>广州·第五届ACBC动漫盛典-二次元游园会</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>广龙路中油BP(白云万顺达南加油站)北侧约260米 李宁运动中心</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2024.01.27 10:00-01.27 17:00</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>619</v>
+          <t>沙滘中路41-50号 火星工厂</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024.01.27 12:00-01.29 00:00</t>
+        </is>
       </c>
       <c r="G13" t="n">
-        <v>60</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79317&amp;msource=Msearch_colligation</t>
+        <v>646</v>
+      </c>
+      <c r="H13" t="n">
+        <v>48</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80415&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2663,33 +2741,32 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>广州·第五人格only唐人街春市</t>
+          <t>广州·蓝锁only2.0</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2024.01.27 10:00-01.27 16:30</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>2033</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>不可售</t>
-        </is>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79038&amp;msource=Msearch_colligation</t>
+          <t>大石街石北工业大道644号 巨大创意产业园</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2024.01.27 10:00-01.27 17:00</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>865</v>
+      </c>
+      <c r="H14" t="n">
+        <v>65</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79750&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2699,36 +2776,37 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024.01.27</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>广州·第五届ACBC动漫盛典-二次元游园会</t>
+          <t>广州·《卡农》世界经典音乐之旅音乐会</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>沙滘中路41-50号 火星工厂</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2024.01.27 12:00-01.29 00:00</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>606</v>
+          <t>东风中路299号 广州中山纪念堂</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2024.01.28 19:00-01.28 21:00</t>
+        </is>
       </c>
       <c r="G15" t="n">
-        <v>48</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80415&amp;msource=Msearch_colligation</t>
+        <v>26</v>
+      </c>
+      <c r="H15" t="n">
+        <v>100</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80047&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2738,36 +2816,37 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024.01.27</t>
+          <t>2024.01.28</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>广州·蓝锁only2.0</t>
+          <t>广州·文豪野犬only</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>大石街石北工业大道644号 巨大创意产业园</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2024.01.27 10:00-01.27 17:00</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>757</v>
+          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2024.01.28 10:00-01.28 17:00</t>
+        </is>
       </c>
       <c r="G16" t="n">
-        <v>65</v>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79750&amp;msource=Msearch_colligation</t>
+        <v>467</v>
+      </c>
+      <c r="H16" t="n">
+        <v>60</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80436&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2777,36 +2856,37 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.01.29</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>广州·《卡农》世界经典音乐之旅音乐会</t>
+          <t>广州·排球少年.only</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>东风中路299号 广州中山纪念堂</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2024.01.28 19:00-01.28 21:00</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>20</v>
+          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2024.01.29 10:00-01.29 17:00</t>
+        </is>
       </c>
       <c r="G17" t="n">
-        <v>100</v>
-      </c>
-      <c r="H17" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80047&amp;msource=Msearch_colligation</t>
+        <v>345</v>
+      </c>
+      <c r="H17" t="n">
+        <v>60</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80453&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2816,12 +2896,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.01.30</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>广州·排球少年.only</t>
+          <t>广州·进击的巨人only</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2829,23 +2909,24 @@
           <t>奥体南路12号 优托邦(奥体旗舰店)</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2024.01.28 10:00-01.28 17:00</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>247</v>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2024.01.30 10:00-01.30 17:00</t>
+        </is>
       </c>
       <c r="G18" t="n">
+        <v>381</v>
+      </c>
+      <c r="H18" t="n">
         <v>60</v>
       </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80453&amp;msource=Msearch_colligation</t>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80454&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2855,36 +2936,37 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024.01.28</t>
+          <t>2024.02.01</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>广州·文豪野犬only</t>
+          <t>广州·U.M.A闪耀ONLY（马娘only）</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2024.01.28 10:00-01.28 17:00</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>332</v>
+          <t>东圃中山大道中358号 轰谧斯酒店</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2024.02.01 10:00-02.01 17:00</t>
+        </is>
       </c>
       <c r="G19" t="n">
-        <v>60</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80436&amp;msource=Msearch_colligation</t>
+        <v>351</v>
+      </c>
+      <c r="H19" t="n">
+        <v>68</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80184&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2894,36 +2976,37 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024.01.30</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>广州·进击的巨人only</t>
+          <t>从化·FS动漫展</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2024.01.30 10:00-01.30 17:00</t>
-        </is>
-      </c>
-      <c r="F20" t="n">
-        <v>310</v>
+          <t>从城大道383号 云岭湖酒店</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2024.02.03 10:00-02.03 17:00</t>
+        </is>
       </c>
       <c r="G20" t="n">
-        <v>60</v>
-      </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80454&amp;msource=Msearch_colligation</t>
+        <v>1118</v>
+      </c>
+      <c r="H20" t="n">
+        <v>35</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=77976&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2933,36 +3016,37 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024.02.01</t>
+          <t>2024.02.03</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>广州·U.M.A闪耀ONLY（马娘only）</t>
+          <t>广州·怀旧ONLY</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>东圃中山大道中358号 轰谧斯酒店</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2024.02.01 10:00-02.01 17:00</t>
-        </is>
-      </c>
-      <c r="F21" t="n">
-        <v>292</v>
+          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2024.02.03 10:00-02.03 16:30</t>
+        </is>
       </c>
       <c r="G21" t="n">
-        <v>68</v>
-      </c>
-      <c r="H21" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80184&amp;msource=Msearch_colligation</t>
+        <v>489</v>
+      </c>
+      <c r="H21" t="n">
+        <v>60</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79752&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -2972,36 +3056,37 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024.02.03</t>
+          <t>2024.02.04</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>从化·FS动漫展</t>
+          <t>广州·次元LAB 二次元电音节</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>从城大道383号 云岭湖酒店</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2024.02.03 10:00-02.03 17:00</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>1025</v>
+          <t>革新路124号 太古仓码头</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2024.02.04 12:30-02.04 21:00</t>
+        </is>
       </c>
       <c r="G22" t="n">
-        <v>35</v>
-      </c>
-      <c r="H22" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=77976&amp;msource=Msearch_colligation</t>
+        <v>760</v>
+      </c>
+      <c r="H22" t="n">
+        <v>380</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80147&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3011,36 +3096,37 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024.02.03</t>
+          <t>2024.02.12</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>广州·怀旧ONLY</t>
+          <t>广州·EY动漫嘉年华</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>洛浦街厦滘西环路1号 广州市岭南国际电子商务会展中心</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2024.02.03 10:00-02.03 16:30</t>
-        </is>
-      </c>
-      <c r="F23" t="n">
-        <v>398</v>
+          <t>机场路1399号广州百信广场二期 李宁运动中心</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2024.02.12 10:00-02.12 17:00</t>
+        </is>
       </c>
       <c r="G23" t="n">
-        <v>75</v>
-      </c>
-      <c r="H23" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79752&amp;msource=Msearch_colligation</t>
+        <v>872</v>
+      </c>
+      <c r="H23" t="n">
+        <v>63</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80574&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3050,36 +3136,37 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024.02.04</t>
+          <t>2024.02.14</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>广州·次元LAB 二次元电音节</t>
+          <t>广州·运动番only4.0</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>革新路124号 太古仓码头</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2024.02.04 12:30-02.04 21:00</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>661</v>
+          <t>洛浦街厦滘西环路1号 岭南会展中心</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2024.02.14 10:00-02.14 17:00</t>
+        </is>
       </c>
       <c r="G24" t="n">
-        <v>380</v>
-      </c>
-      <c r="H24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80147&amp;msource=Msearch_colligation</t>
+        <v>338</v>
+      </c>
+      <c r="H24" t="n">
+        <v>60</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80499&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3089,36 +3176,37 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024.02.12</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>广州·EY动漫嘉年华</t>
+          <t>广州· 妖都原神only 2.0-提瓦特新春游园会</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>机场路1399号广州百信广场二期 李宁运动中心</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>2024.02.12 10:00-02.12 17:00</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>95</v>
+          <t>洛浦街厦滘西环路1号 岭南会展中心</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2024.02.16 09:30-02.16 16:30</t>
+        </is>
       </c>
       <c r="G25" t="n">
-        <v>63</v>
-      </c>
-      <c r="H25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80574&amp;msource=Msearch_colligation</t>
+        <v>523</v>
+      </c>
+      <c r="H25" t="n">
+        <v>58</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79914&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3128,36 +3216,37 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024.02.14</t>
+          <t>2024.02.16</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>广州·运动番only4.0</t>
+          <t>广州·樱漫动漫嘉年华8.0</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>洛浦街厦滘西环路1号 岭南会展中心</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>2024.02.14 10:00-02.14 17:00</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>223</v>
+          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2024.02.16 10:00-02.17 17:00</t>
+        </is>
       </c>
       <c r="G26" t="n">
-        <v>60</v>
-      </c>
-      <c r="H26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80499&amp;msource=Msearch_colligation</t>
+        <v>823</v>
+      </c>
+      <c r="H26" t="n">
+        <v>58</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79792&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3167,36 +3256,37 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.18</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>广州· 妖都原神only 2.0-提瓦特新春游园会</t>
+          <t>广州·cooperative kingdom同人展2.0</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>洛浦街厦滘西环路1号 岭南会展中心</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2024.02.16 09:30-02.16 16:30</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>457</v>
+          <t>洛浦街夏滘西环路1号 岭南电商园</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2024.02.18 10:00-02.18 17:00</t>
+        </is>
       </c>
       <c r="G27" t="n">
-        <v>58</v>
-      </c>
-      <c r="H27" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79914&amp;msource=Msearch_colligation</t>
+        <v>847</v>
+      </c>
+      <c r="H27" t="n">
+        <v>55</v>
+      </c>
+      <c r="I27" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79264&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3206,36 +3296,37 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024.02.16</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>广州·樱漫动漫嘉年华8.0</t>
+          <t>广州·SISP动漫游戏嘉年华</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>奥体南路12号 优托邦(奥体旗舰店)</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>2024.02.16 10:00-02.17 17:00</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
-        <v>685</v>
+          <t>西湾路150号 悦汇城</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2024.02.24 13:00-02.25 19:00</t>
+        </is>
       </c>
       <c r="G28" t="n">
-        <v>58</v>
-      </c>
-      <c r="H28" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79792&amp;msource=Msearch_colligation</t>
+        <v>66</v>
+      </c>
+      <c r="H28" t="n">
+        <v>48</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80624&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3245,36 +3336,37 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024.02.18</t>
+          <t>2024.02.24</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>广州·cooperative kingdom同人展2.0</t>
+          <t>广州·砂糖桔动漫荟STJ01</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>洛浦街夏滘西环路1号 岭南电商园</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2024.02.18 10:00-02.18 17:00</t>
-        </is>
-      </c>
-      <c r="F29" t="n">
-        <v>801</v>
+          <t>东沙大道16号 广州国际医药港</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2024.02.24 10:00-02.25 18:00</t>
+        </is>
       </c>
       <c r="G29" t="n">
-        <v>55</v>
-      </c>
-      <c r="H29" t="b">
-        <v>0</v>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79264&amp;msource=Msearch_colligation</t>
+        <v>87</v>
+      </c>
+      <c r="H29" t="n">
+        <v>60</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80774&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3289,31 +3381,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>广州·SISP动漫游戏嘉年华</t>
+          <t>广州黄龄【有没有吃过饭】LIVEHOUSE巡演—广州站</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>西湾路150号 悦汇城</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2024.02.24 13:00-02.25 19:00</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>10</v>
+          <t>新港东路磨碟沙大街118号第8栋 媒棚LIVE</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2024.02.24 20:00-02.24 22:00</t>
+        </is>
       </c>
       <c r="G30" t="n">
-        <v>48</v>
-      </c>
-      <c r="H30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80624&amp;msource=Msearch_colligation</t>
+        <v>13</v>
+      </c>
+      <c r="H30" t="n">
+        <v>420</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80205&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3323,36 +3416,37 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024.02.24</t>
+          <t>2024.02.25</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>广州黄龄【有没有吃过饭】LIVEHOUSE巡演—广州站</t>
+          <t>广州·第五届清云动漫展</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>新港东路磨碟沙大街118号第8栋 媒棚LIVE</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2024.02.24 20:00-02.24 22:00</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>10</v>
+          <t>丰乐北路898号 雅居乐黄埔创新中心</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2024.02.25 10:00-02.25 17:00</t>
+        </is>
       </c>
       <c r="G31" t="n">
-        <v>420</v>
-      </c>
-      <c r="H31" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80205&amp;msource=Msearch_colligation</t>
+        <v>90</v>
+      </c>
+      <c r="H31" t="n">
+        <v>40</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80502&amp;msource=Msearch_colligation</t>
         </is>
       </c>
     </row>
@@ -3375,21 +3469,22 @@
           <t>清河东路288号 科尔海悦酒店</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
         <is>
           <t>2024.03.02 10:00-03.02 17:00</t>
         </is>
       </c>
-      <c r="F32" t="n">
-        <v>185</v>
-      </c>
       <c r="G32" t="n">
+        <v>220</v>
+      </c>
+      <c r="H32" t="n">
         <v>60</v>
       </c>
-      <c r="H32" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" t="inlineStr">
+      <c r="I32" t="b">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80271&amp;msource=Msearch_colligation</t>
         </is>
@@ -3414,21 +3509,22 @@
           <t>清河东路288号 科尔海悦酒店</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
         <is>
           <t>2024.03.16 10:00-03.16 21:00</t>
         </is>
       </c>
-      <c r="F33" t="n">
-        <v>474</v>
-      </c>
       <c r="G33" t="n">
+        <v>553</v>
+      </c>
+      <c r="H33" t="n">
         <v>39</v>
       </c>
-      <c r="H33" t="b">
-        <v>0</v>
-      </c>
-      <c r="I33" t="inlineStr">
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=79828&amp;msource=Msearch_colligation</t>
         </is>
@@ -3453,21 +3549,22 @@
           <t>洛浦街夏滘西环路1号(厦滘地铁站A口步行290米) 厦喾岭南电商园会展中心</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
         <is>
           <t>2024.03.16 10:00-03.16 17:00</t>
         </is>
       </c>
-      <c r="F34" t="n">
-        <v>1</v>
-      </c>
       <c r="G34" t="n">
+        <v>80</v>
+      </c>
+      <c r="H34" t="n">
         <v>60</v>
       </c>
-      <c r="H34" t="b">
-        <v>0</v>
-      </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80715&amp;msource=Msearch_colligation</t>
         </is>
@@ -3492,21 +3589,22 @@
           <t>机场路1399号广州百信广场二期 李宁运动中心</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
         <is>
           <t>2024.03.23 10:00-03.23 17:00</t>
         </is>
       </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
       <c r="G35" t="n">
+        <v>33</v>
+      </c>
+      <c r="H35" t="n">
         <v>60</v>
       </c>
-      <c r="H35" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" t="inlineStr">
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80716&amp;msource=Msearch_colligation</t>
         </is>
@@ -3531,21 +3629,22 @@
           <t>同泰路颐和山庄 颐和大酒店</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr">
         <is>
           <t>2024.04.20 10:00-04.20 17:00</t>
         </is>
       </c>
-      <c r="F36" t="n">
-        <v>217</v>
-      </c>
       <c r="G36" t="n">
+        <v>266</v>
+      </c>
+      <c r="H36" t="n">
         <v>69</v>
       </c>
-      <c r="H36" t="b">
-        <v>0</v>
-      </c>
-      <c r="I36" t="inlineStr">
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="inlineStr">
         <is>
           <t>https://show.bilibili.com/platform/detail.html?id=80282&amp;msource=Msearch_colligation</t>
         </is>
@@ -3563,6 +3662,7 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -3576,6 +3676,7 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -3594,6 +3695,7 @@
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>